<commit_message>
:bug: Fix the merge excel error
</commit_message>
<xml_diff>
--- a/sample/merge/merge_writer.xlsx
+++ b/sample/merge/merge_writer.xlsx
@@ -14,13 +14,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
+    <t>数据2</t>
+  </si>
+  <si>
     <t>数据1</t>
   </si>
   <si>
-    <t>数据2</t>
+    <t>数据3</t>
   </si>
   <si>
-    <t>数据3</t>
+    <t>密码</t>
   </si>
   <si>
     <t>名字</t>
@@ -29,10 +32,10 @@
     <t>描述</t>
   </si>
   <si>
-    <t>密码</t>
+    <t>邮箱</t>
   </si>
   <si>
-    <t>邮箱</t>
+    <t>123456</t>
   </si>
   <si>
     <t>小明</t>
@@ -41,19 +44,16 @@
     <t>数学好</t>
   </si>
   <si>
-    <t>123456</t>
+    <t>xiaomi@example.com</t>
   </si>
   <si>
-    <t>xiaomi@example.com</t>
+    <t>456789</t>
   </si>
   <si>
     <t>小红</t>
   </si>
   <si>
     <t>语文好</t>
-  </si>
-  <si>
-    <t>456789</t>
   </si>
   <si>
     <t>xiaohong@example.com</t>
@@ -111,7 +111,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -162,7 +162,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>